<commit_message>
some data files updated/created and docs
</commit_message>
<xml_diff>
--- a/rapports et jdt/JdT_nithujan.xlsx
+++ b/rapports et jdt/JdT_nithujan.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPA\TPI-astronomie\rapports et jdt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\rapports et jdt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C49F2AC-8570-4F74-9B75-76FC3B30F2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -283,24 +282,60 @@
     <t>Gestion erreurs login form</t>
   </si>
   <si>
-    <t>terminée</t>
-  </si>
-  <si>
     <t>Extraction données csv</t>
   </si>
   <si>
     <t>à terminer : renommage des fichiers unique / données objets célestes</t>
+  </si>
+  <si>
+    <t>ajouter les indications de login réussie: login -&gt; logout, menu réservé aux admins</t>
+  </si>
+  <si>
+    <t>Gestion des login</t>
+  </si>
+  <si>
+    <t>Terminée</t>
+  </si>
+  <si>
+    <t>Recherche et ajout d'un logo au header</t>
+  </si>
+  <si>
+    <t>Terminé</t>
+  </si>
+  <si>
+    <t>Faire des tests plus précis pour la recherche dans la liste</t>
+  </si>
+  <si>
+    <t>Maquette de la page du catalogue Messier</t>
+  </si>
+  <si>
+    <t>Question sur les filtres: recherche textuel sur tous les champs ou champs de recherche pour chaque colonnes / réponse: une barre de recherche pour toutes les colonnes = ok / maquette terminée</t>
+  </si>
+  <si>
+    <t>Recherche sur un moyen d'importer les données</t>
+  </si>
+  <si>
+    <t>Correction d'une erreur sur le MLD</t>
+  </si>
+  <si>
+    <t>note: difficle de changer l'ordre des colonnes dans l'ERD tool de pgAdmin 4 -&gt; chmgnt manuel sur le script SQL</t>
+  </si>
+  <si>
+    <t>Dossier de projet</t>
+  </si>
+  <si>
+    <t>Image générée pour MLD pose problème -&gt; à refaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +361,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -401,31 +443,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,966 +778,1176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="61.5546875" customWidth="1"/>
-    <col min="7" max="7" width="85.44140625" customWidth="1"/>
-    <col min="8" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="61.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="85.42578125" style="5" customWidth="1"/>
+    <col min="8" max="9" width="18.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="18" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D2" s="14" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>44683</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="8">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="8">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="9">
         <f>C5-B5</f>
         <v>6.9444444444444198E-3</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="8">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="9">
         <f t="shared" ref="D6:D31" si="0">C6-B6</f>
         <v>9.3749999999999944E-2</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="8">
         <v>0.5625</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="8">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="9">
         <f t="shared" si="0"/>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="8">
         <v>0.61458333333333337</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="8">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="9">
         <f t="shared" si="0"/>
         <v>1.388888888888884E-2</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>44684</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="8">
         <v>0.375</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="8">
         <v>0.375</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="9">
         <f t="shared" si="0"/>
         <v>2.430555555555558E-2</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="8">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="8">
         <v>0.4201388888888889</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="9">
         <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="8">
         <v>0.4201388888888889</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="8">
         <v>0.4375</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="9">
         <f t="shared" si="0"/>
         <v>1.7361111111111105E-2</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="8">
         <v>0.4375</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="8">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="9">
         <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="8">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="8">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="9">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="8">
         <v>0.48958333333333331</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="9">
         <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="8">
         <v>0.5625</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="8">
         <v>0.62152777777777779</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="9">
         <f t="shared" si="0"/>
         <v>5.902777777777779E-2</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="8">
         <v>0.625</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="8">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="9">
         <f t="shared" si="0"/>
         <v>6.9444444444444198E-3</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="3">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="8">
         <v>0.63194444444444442</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="8">
         <v>0.63541666666666663</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="9">
         <f t="shared" si="0"/>
         <v>3.4722222222222099E-3</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="8">
         <v>0.63541666666666663</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="9">
         <f t="shared" si="0"/>
         <v>1.0416666666666741E-2</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="8">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="9">
         <f t="shared" si="0"/>
         <v>2.0833333333333259E-2</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="8">
         <v>0.6875</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="9">
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
         <v>44685</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="8">
         <v>0.36805555555555558</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="9">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="8">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="8">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="9">
         <f t="shared" si="0"/>
         <v>1.7361111111111049E-2</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="E25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="3">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="8">
         <v>0.42708333333333331</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="8">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="9">
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="E26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="8">
         <v>0.44791666666666669</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="9">
         <f t="shared" si="0"/>
         <v>6.2499999999999944E-2</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="E27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="8">
         <v>0.5625</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="8">
         <v>0.57291666666666663</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="9">
         <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="8">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="8">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="9">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="8">
         <v>0.60416666666666663</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="8">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="9">
         <f t="shared" si="0"/>
         <v>2.430555555555558E-2</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="8">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="9">
         <f t="shared" si="0"/>
         <v>2.7777777777777679E-2</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="8">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="9">
         <f t="shared" ref="D32" si="1">C32-B32</f>
         <v>3.125E-2</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="8">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="8">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="9">
         <f t="shared" ref="D33" si="2">C33-B33</f>
         <v>6.9444444444445308E-3</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
         <v>44686</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="8">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="9">
         <f t="shared" ref="D35" si="3">C35-B35</f>
         <v>6.5972222222222265E-2</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="8">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="9">
         <f t="shared" ref="D36:D39" si="4">C36-B36</f>
         <v>0.10069444444444436</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="3">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="8">
         <v>0.5625</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="8">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="9">
         <f t="shared" si="4"/>
         <v>4.8611111111111049E-2</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="8">
         <v>0.61111111111111105</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="8">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="9">
         <f t="shared" si="4"/>
         <v>1.736111111111116E-2</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
-      <c r="B39" s="3">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="8">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="8">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="9">
         <f t="shared" si="4"/>
         <v>3.819444444444442E-2</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="8">
         <v>0.67708333333333337</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="8">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="9">
         <f t="shared" ref="D40" si="5">C40-B40</f>
         <v>2.777777777777779E-2</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="15" t="s">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
         <v>44690</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="8">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="8">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="9">
         <f t="shared" ref="D42:D43" si="6">C42-B42</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="8">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="8">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="9">
         <f t="shared" si="6"/>
         <v>4.8611111111111105E-2</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="3">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="8">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="8">
         <v>0.5</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="9">
         <f t="shared" ref="D44:D45" si="7">C44-B44</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="1" t="s">
+      <c r="E44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="8">
         <v>0.5</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="9">
         <f t="shared" si="7"/>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="8">
         <v>0.5625</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="8">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="9">
         <f t="shared" ref="D46" si="8">C46-B46</f>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="3">
+      <c r="G46" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="8">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="8">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="9">
         <f t="shared" ref="D47" si="9">C47-B47</f>
         <v>4.513888888888884E-2</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>84</v>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>44691</v>
+      </c>
+      <c r="B49" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C49" s="8">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D49" s="9">
+        <f t="shared" ref="D49" si="10">C49-B49</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="8">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C50" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="D50" s="9">
+        <f t="shared" ref="D50" si="11">C50-B50</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="C51" s="8">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D51" s="9">
+        <f t="shared" ref="D51" si="12">C51-B51</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="8">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C52" s="8">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D52" s="9">
+        <f t="shared" ref="D52" si="13">C52-B52</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="8">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C53" s="8">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D53" s="9">
+        <f t="shared" ref="D53:D54" si="14">C53-B53</f>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="8">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C54" s="8">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D54" s="9">
+        <f t="shared" si="14"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="C55" s="8">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D55" s="9">
+        <f t="shared" ref="D55" si="15">C55-B55</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="8">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C56" s="8">
+        <v>0.65625</v>
+      </c>
+      <c r="D56" s="9">
+        <f t="shared" ref="D56" si="16">C56-B56</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="8">
+        <v>0.65625</v>
+      </c>
+      <c r="C57" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D57" s="9">
+        <f t="shared" ref="D57" si="17">C57-B57</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1679,6 +1956,6 @@
     <mergeCell ref="D2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="66" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data files update and some docs
</commit_message>
<xml_diff>
--- a/rapports et jdt/JdT_nithujan.xlsx
+++ b/rapports et jdt/JdT_nithujan.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -325,6 +325,42 @@
   </si>
   <si>
     <t>Image générée pour MLD pose problème -&gt; à refaire</t>
+  </si>
+  <si>
+    <t>Màj de la db pour faciliter l'import des données</t>
+  </si>
+  <si>
+    <t>mld à recréer / utilisation de fichier backup au lieu de .sql pour créer la db / type de colonne changé pour celestial_object.right_ascension</t>
+  </si>
+  <si>
+    <t>fichier csv erroné: m45 n'a pas de n° ngc --&gt; son nom commun a été pris --&gt; modif. csv ??</t>
+  </si>
+  <si>
+    <t>Création du script permettant de remplir la table celestiabl_object</t>
+  </si>
+  <si>
+    <t>Téléchargement d'images pour la bdd</t>
+  </si>
+  <si>
+    <t>httrack est trop long --&gt; extension firefox DownThemAll lien: http://www.httrack.com/page/2/fr/index.html</t>
+  </si>
+  <si>
+    <t>Extension Firefox: DownThemAll -&gt; réussite ! Choisir jpg ET png / suite: renommer les images utiles pour le site</t>
+  </si>
+  <si>
+    <t>Création d'un script pour rename le images</t>
+  </si>
+  <si>
+    <t>src: https://stackoverflow.com/questions/40904836/how-to-get-n-files-in-a-directory-order-by-last-modified-date -- https://stackoverflow.com/questions/52152228/how-to-filter-a-list-with-a-list-of-strings-in-powershell -- https://stackoverflow.com/questions/11816218/renaming-files-in-powershell-using-the-folder-name -- https://stackoverflow.com/questions/51818485/increment-variable-in-powershell-from-within-if-statement-within-a-foreach-loop</t>
+  </si>
+  <si>
+    <t>Script créé mais impossible de renommer les images --&gt; à terminer</t>
+  </si>
+  <si>
+    <t>Questions à poser à la cdp dans fichiers /analyse/questions.txt</t>
+  </si>
+  <si>
+    <t>Mise à jour du dossier de projet</t>
   </si>
 </sst>
 </file>
@@ -451,17 +487,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -492,6 +519,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -782,78 +818,78 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G57"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="61.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="85.42578125" style="5" customWidth="1"/>
-    <col min="8" max="9" width="18.7109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="18" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="9.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="61.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="85.42578125" style="3" customWidth="1"/>
+    <col min="8" max="9" width="18.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>44683</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="5">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <f>C5-B5</f>
         <v>6.9444444444444198E-3</v>
       </c>
@@ -868,14 +904,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="8">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <f t="shared" ref="D6:D31" si="0">C6-B6</f>
         <v>9.3749999999999944E-2</v>
       </c>
@@ -890,14 +926,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="8">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>5.208333333333337E-2</v>
       </c>
@@ -912,14 +948,14 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5">
         <v>0.61458333333333337</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>1.388888888888884E-2</v>
       </c>
@@ -934,25 +970,25 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>44684</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>0.375</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
@@ -967,14 +1003,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="8">
+      <c r="A11" s="7"/>
+      <c r="B11" s="5">
         <v>0.375</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>2.430555555555558E-2</v>
       </c>
@@ -989,14 +1025,14 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="8">
+      <c r="A12" s="7"/>
+      <c r="B12" s="5">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="5">
         <v>0.4201388888888889</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
@@ -1011,14 +1047,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="8">
+      <c r="A13" s="7"/>
+      <c r="B13" s="5">
         <v>0.4201388888888889</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>0.4375</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>1.7361111111111105E-2</v>
       </c>
@@ -1033,14 +1069,14 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="8">
+      <c r="A14" s="7"/>
+      <c r="B14" s="5">
         <v>0.4375</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
@@ -1055,14 +1091,14 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="8">
+      <c r="A15" s="7"/>
+      <c r="B15" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="6">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
@@ -1077,14 +1113,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="8">
+      <c r="A16" s="7"/>
+      <c r="B16" s="5">
         <v>0.48958333333333331</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="6">
         <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
@@ -1099,14 +1135,14 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="8">
+      <c r="A17" s="7"/>
+      <c r="B17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="5">
         <v>0.62152777777777779</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="6">
         <f t="shared" si="0"/>
         <v>5.902777777777779E-2</v>
       </c>
@@ -1121,14 +1157,14 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="8">
+      <c r="A18" s="7"/>
+      <c r="B18" s="5">
         <v>0.625</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="5">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="6">
         <f t="shared" si="0"/>
         <v>6.9444444444444198E-3</v>
       </c>
@@ -1143,14 +1179,14 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="8">
+      <c r="A19" s="7"/>
+      <c r="B19" s="5">
         <v>0.63194444444444442</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="5">
         <v>0.63541666666666663</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="6">
         <f t="shared" si="0"/>
         <v>3.4722222222222099E-3</v>
       </c>
@@ -1165,14 +1201,14 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="8">
+      <c r="A20" s="7"/>
+      <c r="B20" s="5">
         <v>0.63541666666666663</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="5">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="6">
         <f t="shared" si="0"/>
         <v>1.0416666666666741E-2</v>
       </c>
@@ -1187,14 +1223,14 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="8">
+      <c r="A21" s="7"/>
+      <c r="B21" s="5">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="6">
         <f t="shared" si="0"/>
         <v>2.0833333333333259E-2</v>
       </c>
@@ -1209,14 +1245,14 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="8">
+      <c r="A22" s="7"/>
+      <c r="B22" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="5">
         <v>0.6875</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="6">
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
@@ -1231,25 +1267,25 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="7">
         <v>44685</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="5">
         <v>0.36805555555555558</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="6">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
@@ -1264,14 +1300,14 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="8">
+      <c r="A25" s="7"/>
+      <c r="B25" s="5">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="6">
         <f t="shared" si="0"/>
         <v>1.7361111111111049E-2</v>
       </c>
@@ -1286,14 +1322,14 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="8">
+      <c r="A26" s="7"/>
+      <c r="B26" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="6">
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
@@ -1308,14 +1344,14 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="8">
+      <c r="A27" s="7"/>
+      <c r="B27" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="6">
         <f t="shared" si="0"/>
         <v>6.2499999999999944E-2</v>
       </c>
@@ -1330,14 +1366,14 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="8">
+      <c r="A28" s="7"/>
+      <c r="B28" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="5">
         <v>0.57291666666666663</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="6">
         <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
@@ -1352,14 +1388,14 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="8">
+      <c r="A29" s="7"/>
+      <c r="B29" s="5">
         <v>0.57291666666666663</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="5">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="6">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
@@ -1374,14 +1410,14 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="8">
+      <c r="A30" s="7"/>
+      <c r="B30" s="5">
         <v>0.60416666666666663</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="6">
         <f t="shared" si="0"/>
         <v>2.430555555555558E-2</v>
       </c>
@@ -1396,14 +1432,14 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="8">
+      <c r="A31" s="7"/>
+      <c r="B31" s="5">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="6">
         <f t="shared" si="0"/>
         <v>2.7777777777777679E-2</v>
       </c>
@@ -1418,14 +1454,14 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="8">
+      <c r="A32" s="7"/>
+      <c r="B32" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="5">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="6">
         <f t="shared" ref="D32" si="1">C32-B32</f>
         <v>3.125E-2</v>
       </c>
@@ -1440,14 +1476,14 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="8">
+      <c r="A33" s="7"/>
+      <c r="B33" s="5">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="5">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="6">
         <f t="shared" ref="D33" si="2">C33-B33</f>
         <v>6.9444444444445308E-3</v>
       </c>
@@ -1460,25 +1496,25 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+      <c r="A35" s="7">
         <v>44686</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="6">
         <f t="shared" ref="D35" si="3">C35-B35</f>
         <v>6.5972222222222265E-2</v>
       </c>
@@ -1493,14 +1529,14 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="8">
+      <c r="A36" s="7"/>
+      <c r="B36" s="5">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="6">
         <f t="shared" ref="D36:D39" si="4">C36-B36</f>
         <v>0.10069444444444436</v>
       </c>
@@ -1513,14 +1549,14 @@
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="8">
+      <c r="A37" s="7"/>
+      <c r="B37" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="5">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="6">
         <f t="shared" si="4"/>
         <v>4.8611111111111049E-2</v>
       </c>
@@ -1535,14 +1571,14 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="8">
+      <c r="A38" s="7"/>
+      <c r="B38" s="5">
         <v>0.61111111111111105</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="6">
         <f t="shared" si="4"/>
         <v>1.736111111111116E-2</v>
       </c>
@@ -1555,14 +1591,14 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="8">
+      <c r="A39" s="7"/>
+      <c r="B39" s="5">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="5">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="6">
         <f t="shared" si="4"/>
         <v>3.819444444444442E-2</v>
       </c>
@@ -1577,14 +1613,14 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="8">
+      <c r="A40" s="7"/>
+      <c r="B40" s="5">
         <v>0.67708333333333337</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="5">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="6">
         <f t="shared" ref="D40" si="5">C40-B40</f>
         <v>2.777777777777779E-2</v>
       </c>
@@ -1597,27 +1633,27 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
+      <c r="A42" s="7">
         <v>44690</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="5">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="5">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="6">
         <f t="shared" ref="D42:D43" si="6">C42-B42</f>
         <v>2.0833333333333315E-2</v>
       </c>
@@ -1632,14 +1668,14 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="8">
+      <c r="A43" s="7"/>
+      <c r="B43" s="5">
         <v>0.43055555555555558</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="5">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="6">
         <f t="shared" si="6"/>
         <v>4.8611111111111105E-2</v>
       </c>
@@ -1654,14 +1690,14 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="8">
+      <c r="A44" s="7"/>
+      <c r="B44" s="5">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="5">
         <v>0.5</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="6">
         <f t="shared" ref="D44:D45" si="7">C44-B44</f>
         <v>2.0833333333333315E-2</v>
       </c>
@@ -1676,14 +1712,14 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="8">
+      <c r="A45" s="7"/>
+      <c r="B45" s="5">
         <v>0.5</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="6">
         <f t="shared" si="7"/>
         <v>1.041666666666663E-2</v>
       </c>
@@ -1698,14 +1734,14 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="8">
+      <c r="A46" s="7"/>
+      <c r="B46" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="6">
         <f t="shared" ref="D46" si="8">C46-B46</f>
         <v>2.083333333333337E-2</v>
       </c>
@@ -1720,14 +1756,14 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="8">
+      <c r="A47" s="7"/>
+      <c r="B47" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="6">
         <f t="shared" ref="D47" si="9">C47-B47</f>
         <v>4.513888888888884E-2</v>
       </c>
@@ -1742,25 +1778,25 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
+      <c r="A49" s="7">
         <v>44691</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="5">
         <v>0.36458333333333331</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="6">
         <f t="shared" ref="D49" si="10">C49-B49</f>
         <v>3.125E-2</v>
       </c>
@@ -1775,14 +1811,14 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="8">
+      <c r="A50" s="7"/>
+      <c r="B50" s="5">
         <v>0.36458333333333331</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="5">
         <v>0.375</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="6">
         <f t="shared" ref="D50" si="11">C50-B50</f>
         <v>1.0416666666666685E-2</v>
       </c>
@@ -1797,14 +1833,14 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="8">
+      <c r="A51" s="7"/>
+      <c r="B51" s="5">
         <v>0.375</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="6">
         <f t="shared" ref="D51" si="12">C51-B51</f>
         <v>2.430555555555558E-2</v>
       </c>
@@ -1819,14 +1855,14 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="8">
+      <c r="A52" s="7"/>
+      <c r="B52" s="5">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="6">
         <f t="shared" ref="D52" si="13">C52-B52</f>
         <v>6.9444444444444198E-3</v>
       </c>
@@ -1841,14 +1877,14 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="8">
+      <c r="A53" s="7"/>
+      <c r="B53" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="5">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="6">
         <f t="shared" ref="D53:D54" si="14">C53-B53</f>
         <v>7.291666666666663E-2</v>
       </c>
@@ -1863,14 +1899,14 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="B54" s="8">
+      <c r="A54" s="7"/>
+      <c r="B54" s="5">
         <v>0.48958333333333331</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="6">
         <f t="shared" si="14"/>
         <v>2.0833333333333315E-2</v>
       </c>
@@ -1885,14 +1921,14 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="8">
+      <c r="A55" s="7"/>
+      <c r="B55" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="6">
         <f t="shared" ref="D55" si="15">C55-B55</f>
         <v>6.597222222222221E-2</v>
       </c>
@@ -1907,14 +1943,14 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="B56" s="8">
+      <c r="A56" s="7"/>
+      <c r="B56" s="5">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="5">
         <v>0.65625</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="6">
         <f t="shared" ref="D56" si="16">C56-B56</f>
         <v>1.7361111111111049E-2</v>
       </c>
@@ -1929,14 +1965,14 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="8">
+      <c r="A57" s="7"/>
+      <c r="B57" s="5">
         <v>0.65625</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C57" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="6">
         <f t="shared" ref="D57" si="17">C57-B57</f>
         <v>1.041666666666663E-2</v>
       </c>
@@ -1948,6 +1984,169 @@
       </c>
       <c r="G57" s="2" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C59" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D59" s="6">
+        <f t="shared" ref="D59" si="18">C59-B59</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="5">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C60" s="5">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D60" s="6">
+        <f t="shared" ref="D60" si="19">C60-B60</f>
+        <v>7.9861111111111049E-2</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="C61" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D61" s="6">
+        <f t="shared" ref="D61" si="20">C61-B61</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C62" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="D62" s="6">
+        <f t="shared" ref="D62" si="21">C62-B62</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C63" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D63" s="6">
+        <f t="shared" ref="D63" si="22">C63-B63</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C64" s="5">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D64" s="6">
+        <f t="shared" ref="D64" si="23">C64-B64</f>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="5">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C65" s="5">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D65" s="6">
+        <f t="shared" ref="D65" si="24">C65-B65</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor updates and some files moved
</commit_message>
<xml_diff>
--- a/rapports et jdt/JdT_nithujan.xlsx
+++ b/rapports et jdt/JdT_nithujan.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="127">
   <si>
     <t>Date</t>
   </si>
@@ -361,6 +361,60 @@
   </si>
   <si>
     <t>Mise à jour du dossier de projet</t>
+  </si>
+  <si>
+    <t>autre site que wikipedia utilisé: https://www.messier-objects.com/messier-catalogue/ -- ces images ont des noms qui permetttent de faciliter le renommage</t>
+  </si>
+  <si>
+    <t>Import des images  des éléments de la bdd en local</t>
+  </si>
+  <si>
+    <t>Création d'un script Powershell pour extraire les noms des images dans un csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fichiers: get-pictures-cvs.ps1, pictures.csv et images dans /assets -; src: https://docs.microsoft.com/en-us/powershell/module/microsoft.powershell.core/about/about_regular_expressions?view=powershell-7.2 -- https://stackoverflow.com/questions/54882043/powershell-variable-assignment-vs-pipeline -- https://stackoverflow.com/questions/27970441/powershell-string-does-not-contain -- </t>
+  </si>
+  <si>
+    <t>Ajout des données du csv  dans une table temporaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impossible à faire erreur d'encodage </t>
+  </si>
+  <si>
+    <t>Encodage changé mais données qui manque dans le csv --&gt; script à changer</t>
+  </si>
+  <si>
+    <t>Correction du script qui créé le fichier csv pour les images</t>
+  </si>
+  <si>
+    <t>regex erroné a été changé / problème d'encodage</t>
+  </si>
+  <si>
+    <t>Discussion avec la cdp pour questions sur mcd/mld</t>
+  </si>
+  <si>
+    <t>Création de la bdd</t>
+  </si>
+  <si>
+    <t>terminée + fichier backup créé</t>
+  </si>
+  <si>
+    <t>tables temp à ne pas inclure mais mettre dans doc/réalisation -- ok de download les images depuis un autre site</t>
+  </si>
+  <si>
+    <t>Réalisation: import des données de la bdd --&gt; à finir</t>
+  </si>
+  <si>
+    <t>Résultats des tests à rédiger</t>
+  </si>
+  <si>
+    <t>Scripts PowerShell</t>
+  </si>
+  <si>
+    <t>vérification et légères modif. effectuées / src: https://stackoverflow.com/questions/4724290/powershell-run-command-from-scripts-directory</t>
+  </si>
+  <si>
+    <t>partie implémentation à faire lire car bcp d'explications</t>
   </si>
 </sst>
 </file>
@@ -818,10 +872,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,6 +2203,257 @@
         <v>107</v>
       </c>
     </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="B67" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C67" s="5">
+        <v>0.34375</v>
+      </c>
+      <c r="D67" s="6">
+        <f t="shared" ref="D67" si="25">C67-B67</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="5">
+        <v>0.34375</v>
+      </c>
+      <c r="C68" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D68" s="6">
+        <f t="shared" ref="D68:D69" si="26">C68-B68</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C69" s="5">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D69" s="6">
+        <f t="shared" si="26"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="5">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C70" s="5">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="D70" s="6">
+        <f t="shared" ref="D70" si="27">C70-B70</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="5">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C71" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D71" s="6">
+        <f t="shared" ref="D71" si="28">C71-B71</f>
+        <v>5.902777777777779E-2</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C72" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D72" s="6">
+        <f t="shared" ref="D72" si="29">C72-B72</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="C73" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D73" s="6">
+        <f t="shared" ref="D73" si="30">C73-B73</f>
+        <v>1.7361111111111105E-2</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
+      <c r="B74" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C74" s="5">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D74" s="6">
+        <f t="shared" ref="D74" si="31">C74-B74</f>
+        <v>-6.9444444444444198E-3</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C75" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D75" s="6">
+        <f t="shared" ref="D75" si="32">C75-B75</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
+      <c r="B76" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C76" s="5">
+        <v>0.65625</v>
+      </c>
+      <c r="D76" s="6">
+        <f t="shared" ref="D76" si="33">C76-B76</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="7"/>
+      <c r="B77" s="5">
+        <v>0.65625</v>
+      </c>
+      <c r="C77" s="5">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D77" s="6">
+        <f t="shared" ref="D77" si="34">C77-B77</f>
+        <v>4.861111111111116E-2</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
new outing started + some docs
</commit_message>
<xml_diff>
--- a/rapports et jdt/JdT_nithujan.xlsx
+++ b/rapports et jdt/JdT_nithujan.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="166">
   <si>
     <t>Date</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Résultat</t>
   </si>
   <si>
-    <t>Réalisé par: Nithujan Jegatheeswaran</t>
-  </si>
-  <si>
     <t>Discussion du cahier des charges avec Mme Andolfatto</t>
   </si>
   <si>
@@ -475,17 +472,108 @@
   </si>
   <si>
     <t>le fichier CSS datatables a été téléchargé en local</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Réalisé pa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Nithujan Jegatheeswaran</t>
+    </r>
+  </si>
+  <si>
+    <t>Temps total (hh:mm):</t>
+  </si>
+  <si>
+    <t>Message d'erreurs plus vague sur la page de login + mise en forme</t>
+  </si>
+  <si>
+    <t>Update du style de la page du catalogue</t>
+  </si>
+  <si>
+    <t>chgmnt dans le fichier css</t>
+  </si>
+  <si>
+    <t>Mise à jour de la planif sur IceScrum</t>
+  </si>
+  <si>
+    <t>Tests écrits et stories terminées marquées done</t>
+  </si>
+  <si>
+    <t>Maquette de la page Nouvelle sortie</t>
+  </si>
+  <si>
+    <t>Maquette créé</t>
+  </si>
+  <si>
+    <t>Création de la classe du formulaire pour les nouvelles sorties</t>
+  </si>
+  <si>
+    <t>à finir: message d'erreurs, validation des champs datetime et time</t>
+  </si>
+  <si>
+    <t>Création de la classe pour les sorties nocturnes</t>
+  </si>
+  <si>
+    <t>Code de la page pour ajouter une nouvelle sortie</t>
+  </si>
+  <si>
+    <t>solution pour les select à rechercher</t>
+  </si>
+  <si>
+    <t>Recerche d'un moyen de bien mettre en forme les éléments html select</t>
+  </si>
+  <si>
+    <t>boostrap-select permet une bonne utilisation des select MAIS nécessite Bootstrap 5</t>
+  </si>
+  <si>
+    <t>Passage de Boostrap 5 à Boostrap 4</t>
+  </si>
+  <si>
+    <t>compliqué car beaucoup de petit chgmnt à faire --&gt; use version beta de boostrap-select</t>
+  </si>
+  <si>
+    <t>Mise en forme de la version beta de bootstrap-select</t>
+  </si>
+  <si>
+    <t>à faire: couleur à changer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="3">
     <numFmt numFmtId="165" formatCode="dd\ mmmm"/>
+    <numFmt numFmtId="168" formatCode="[h]:mm"/>
+    <numFmt numFmtId="169" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +608,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -593,7 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -610,9 +713,6 @@
     <xf numFmtId="20" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -620,9 +720,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
@@ -634,14 +731,23 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -932,10 +1038,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,43 +1059,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="15">
+        <f>SUM(D5:D200)</f>
+        <v>2.7534722222222223</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1003,97 +1116,97 @@
       <c r="C5" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="16">
         <f>C5-B5</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="5">
         <v>0.41666666666666669</v>
       </c>
       <c r="C6" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D6" s="6">
-        <f t="shared" ref="D6:D31" si="0">C6-B6</f>
+      <c r="D6" s="16">
+        <f t="shared" ref="D6:D69" si="0">C6-B6</f>
         <v>9.3749999999999944E-2</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="5">
         <v>0.5625</v>
       </c>
       <c r="C7" s="5">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="16">
         <f t="shared" si="0"/>
         <v>5.208333333333337E-2</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="5">
         <v>0.61458333333333337</v>
       </c>
       <c r="C8" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="16">
         <f t="shared" si="0"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>44684</v>
       </c>
       <c r="B10" s="5">
@@ -1102,295 +1215,295 @@
       <c r="C10" s="5">
         <v>0.375</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="16">
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="5">
         <v>0.375</v>
       </c>
       <c r="C11" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="16">
         <f t="shared" si="0"/>
         <v>2.430555555555558E-2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="5">
         <v>0.40972222222222227</v>
       </c>
       <c r="C12" s="5">
         <v>0.4201388888888889</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="16">
         <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="5">
         <v>0.4201388888888889</v>
       </c>
       <c r="C13" s="5">
         <v>0.4375</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="16">
         <f t="shared" si="0"/>
         <v>1.7361111111111105E-2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="5">
         <v>0.4375</v>
       </c>
       <c r="C14" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="16">
         <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="5">
         <v>0.45833333333333331</v>
       </c>
       <c r="C15" s="5">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="16">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="5">
         <v>0.48958333333333331</v>
       </c>
       <c r="C16" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="16">
         <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="5">
         <v>0.5625</v>
       </c>
       <c r="C17" s="5">
         <v>0.62152777777777779</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="16">
         <f t="shared" si="0"/>
         <v>5.902777777777779E-2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="5">
         <v>0.625</v>
       </c>
       <c r="C18" s="5">
         <v>0.63194444444444442</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="16">
         <f t="shared" si="0"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="5">
         <v>0.63194444444444442</v>
       </c>
       <c r="C19" s="5">
         <v>0.63541666666666663</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="16">
         <f t="shared" si="0"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="5">
         <v>0.63541666666666663</v>
       </c>
       <c r="C20" s="5">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="16">
         <f t="shared" si="0"/>
         <v>1.0416666666666741E-2</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="5">
         <v>0.64583333333333337</v>
       </c>
       <c r="C21" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="16">
         <f t="shared" si="0"/>
         <v>2.0833333333333259E-2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="C22" s="5">
         <v>0.6875</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="16">
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>44685</v>
       </c>
       <c r="B24" s="5">
@@ -1399,227 +1512,227 @@
       <c r="C24" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="16">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="5">
         <v>0.40972222222222227</v>
       </c>
       <c r="C25" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="16">
         <f t="shared" si="0"/>
         <v>1.7361111111111049E-2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="5">
         <v>0.42708333333333331</v>
       </c>
       <c r="C26" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="16">
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="5">
         <v>0.44791666666666669</v>
       </c>
       <c r="C27" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="16">
         <f t="shared" si="0"/>
         <v>6.2499999999999944E-2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="5">
         <v>0.5625</v>
       </c>
       <c r="C28" s="5">
         <v>0.57291666666666663</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="16">
         <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="6"/>
       <c r="B29" s="5">
         <v>0.57291666666666663</v>
       </c>
       <c r="C29" s="5">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="16">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="5">
         <v>0.60416666666666663</v>
       </c>
       <c r="C30" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="16">
         <f t="shared" si="0"/>
         <v>2.430555555555558E-2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="5">
         <v>0.63888888888888895</v>
       </c>
       <c r="C31" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="16">
         <f t="shared" si="0"/>
         <v>2.7777777777777679E-2</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="5">
         <v>0.66666666666666663</v>
       </c>
       <c r="C32" s="5">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D32" s="6">
-        <f t="shared" ref="D32" si="1">C32-B32</f>
+      <c r="D32" s="16">
+        <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="5">
         <v>0.69791666666666663</v>
       </c>
       <c r="C33" s="5">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D33" s="6">
-        <f t="shared" ref="D33" si="2">C33-B33</f>
+      <c r="D33" s="16">
+        <f t="shared" si="0"/>
         <v>6.9444444444445308E-3</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>44686</v>
       </c>
       <c r="B35" s="5">
@@ -1628,137 +1741,137 @@
       <c r="C35" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D35" s="6">
-        <f t="shared" ref="D35" si="3">C35-B35</f>
+      <c r="D35" s="16">
+        <f t="shared" si="0"/>
         <v>6.5972222222222265E-2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="5">
         <v>0.40972222222222227</v>
       </c>
       <c r="C36" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D36" s="6">
-        <f t="shared" ref="D36:D39" si="4">C36-B36</f>
+      <c r="D36" s="16">
+        <f t="shared" si="0"/>
         <v>0.10069444444444436</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="5">
         <v>0.5625</v>
       </c>
       <c r="C37" s="5">
         <v>0.61111111111111105</v>
       </c>
-      <c r="D37" s="6">
-        <f t="shared" si="4"/>
+      <c r="D37" s="16">
+        <f t="shared" si="0"/>
         <v>4.8611111111111049E-2</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="5">
         <v>0.61111111111111105</v>
       </c>
       <c r="C38" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D38" s="6">
-        <f t="shared" si="4"/>
+      <c r="D38" s="16">
+        <f t="shared" si="0"/>
         <v>1.736111111111116E-2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="5">
         <v>0.63888888888888895</v>
       </c>
       <c r="C39" s="5">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D39" s="6">
-        <f t="shared" si="4"/>
+      <c r="D39" s="16">
+        <f t="shared" si="0"/>
         <v>3.819444444444442E-2</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+      <c r="A40" s="6"/>
       <c r="B40" s="5">
         <v>0.67708333333333337</v>
       </c>
       <c r="C40" s="5">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D40" s="6">
-        <f t="shared" ref="D40" si="5">C40-B40</f>
+      <c r="D40" s="16">
+        <f t="shared" si="0"/>
         <v>2.777777777777779E-2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+      <c r="A42" s="6">
         <v>44690</v>
       </c>
       <c r="B42" s="5">
@@ -1767,141 +1880,141 @@
       <c r="C42" s="5">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D42" s="6">
-        <f t="shared" ref="D42:D43" si="6">C42-B42</f>
+      <c r="D42" s="16">
+        <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="6"/>
       <c r="B43" s="5">
         <v>0.43055555555555558</v>
       </c>
       <c r="C43" s="5">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D43" s="6">
-        <f t="shared" si="6"/>
+      <c r="D43" s="16">
+        <f t="shared" si="0"/>
         <v>4.8611111111111105E-2</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="5">
         <v>0.47916666666666669</v>
       </c>
       <c r="C44" s="5">
         <v>0.5</v>
       </c>
-      <c r="D44" s="6">
-        <f t="shared" ref="D44:D45" si="7">C44-B44</f>
+      <c r="D44" s="16">
+        <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
+      <c r="A45" s="6"/>
       <c r="B45" s="5">
         <v>0.5</v>
       </c>
       <c r="C45" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D45" s="6">
-        <f t="shared" si="7"/>
+      <c r="D45" s="16">
+        <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
+      <c r="A46" s="6"/>
       <c r="B46" s="5">
         <v>0.5625</v>
       </c>
       <c r="C46" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D46" s="6">
-        <f t="shared" ref="D46" si="8">C46-B46</f>
+      <c r="D46" s="16">
+        <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
       <c r="B47" s="5">
         <v>0.58333333333333337</v>
       </c>
       <c r="C47" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D47" s="6">
-        <f t="shared" ref="D47" si="9">C47-B47</f>
+      <c r="D47" s="16">
+        <f t="shared" si="0"/>
         <v>4.513888888888884E-2</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="A49" s="6">
         <v>44691</v>
       </c>
       <c r="B49" s="5">
@@ -1910,207 +2023,207 @@
       <c r="C49" s="5">
         <v>0.36458333333333331</v>
       </c>
-      <c r="D49" s="6">
-        <f t="shared" ref="D49" si="10">C49-B49</f>
+      <c r="D49" s="16">
+        <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F49" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
+      <c r="A50" s="6"/>
       <c r="B50" s="5">
         <v>0.36458333333333331</v>
       </c>
       <c r="C50" s="5">
         <v>0.375</v>
       </c>
-      <c r="D50" s="6">
-        <f t="shared" ref="D50" si="11">C50-B50</f>
+      <c r="D50" s="16">
+        <f t="shared" si="0"/>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
+      <c r="A51" s="6"/>
       <c r="B51" s="5">
         <v>0.375</v>
       </c>
       <c r="C51" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D51" s="6">
-        <f t="shared" ref="D51" si="12">C51-B51</f>
+      <c r="D51" s="16">
+        <f t="shared" si="0"/>
         <v>2.430555555555558E-2</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
+      <c r="A52" s="6"/>
       <c r="B52" s="5">
         <v>0.40972222222222227</v>
       </c>
       <c r="C52" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D52" s="6">
-        <f t="shared" ref="D52" si="13">C52-B52</f>
+      <c r="D52" s="16">
+        <f t="shared" si="0"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="6"/>
       <c r="B53" s="5">
         <v>0.41666666666666669</v>
       </c>
       <c r="C53" s="5">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D53" s="6">
-        <f t="shared" ref="D53:D54" si="14">C53-B53</f>
+      <c r="D53" s="16">
+        <f t="shared" si="0"/>
         <v>7.291666666666663E-2</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="6"/>
       <c r="B54" s="5">
         <v>0.48958333333333331</v>
       </c>
       <c r="C54" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D54" s="6">
-        <f t="shared" si="14"/>
+      <c r="D54" s="16">
+        <f t="shared" si="0"/>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="6"/>
       <c r="B55" s="5">
         <v>0.5625</v>
       </c>
       <c r="C55" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D55" s="6">
-        <f t="shared" ref="D55" si="15">C55-B55</f>
+      <c r="D55" s="16">
+        <f t="shared" si="0"/>
         <v>6.597222222222221E-2</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
+      <c r="A56" s="6"/>
       <c r="B56" s="5">
         <v>0.63888888888888895</v>
       </c>
       <c r="C56" s="5">
         <v>0.65625</v>
       </c>
-      <c r="D56" s="6">
-        <f t="shared" ref="D56" si="16">C56-B56</f>
+      <c r="D56" s="16">
+        <f t="shared" si="0"/>
         <v>1.7361111111111049E-2</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G56" s="2" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
+      <c r="A57" s="6"/>
       <c r="B57" s="5">
         <v>0.65625</v>
       </c>
       <c r="C57" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D57" s="6">
-        <f t="shared" ref="D57" si="17">C57-B57</f>
+      <c r="D57" s="16">
+        <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F57" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
+      <c r="A59" s="6">
         <v>44692</v>
       </c>
       <c r="B59" s="5">
@@ -2119,163 +2232,163 @@
       <c r="C59" s="5">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D59" s="6">
-        <f t="shared" ref="D59" si="18">C59-B59</f>
+      <c r="D59" s="16">
+        <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F59" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G59" s="2" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
+      <c r="A60" s="6"/>
       <c r="B60" s="5">
         <v>0.40972222222222227</v>
       </c>
       <c r="C60" s="5">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D60" s="6">
-        <f t="shared" ref="D60" si="19">C60-B60</f>
+      <c r="D60" s="16">
+        <f t="shared" si="0"/>
         <v>7.9861111111111049E-2</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="5">
         <v>0.53125</v>
       </c>
       <c r="C61" s="5">
         <v>0.55208333333333337</v>
       </c>
-      <c r="D61" s="6">
-        <f t="shared" ref="D61" si="20">C61-B61</f>
+      <c r="D61" s="16">
+        <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F61" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
+      <c r="A62" s="6"/>
       <c r="B62" s="5">
         <v>0.55208333333333337</v>
       </c>
       <c r="C62" s="5">
         <v>0.5625</v>
       </c>
-      <c r="D62" s="6">
-        <f t="shared" ref="D62" si="21">C62-B62</f>
+      <c r="D62" s="16">
+        <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
+      <c r="A63" s="6"/>
       <c r="B63" s="5">
         <v>0.5625</v>
       </c>
       <c r="C63" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D63" s="6">
-        <f t="shared" ref="D63" si="22">C63-B63</f>
+      <c r="D63" s="16">
+        <f t="shared" si="0"/>
         <v>6.597222222222221E-2</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
+      <c r="A64" s="6"/>
       <c r="B64" s="5">
         <v>0.63888888888888895</v>
       </c>
       <c r="C64" s="5">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D64" s="6">
-        <f t="shared" ref="D64" si="23">C64-B64</f>
+      <c r="D64" s="16">
+        <f t="shared" si="0"/>
         <v>3.819444444444442E-2</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F64" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+      <c r="A65" s="6"/>
       <c r="B65" s="5">
         <v>0.67708333333333337</v>
       </c>
       <c r="C65" s="5">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D65" s="6">
-        <f t="shared" ref="D65" si="24">C65-B65</f>
+      <c r="D65" s="16">
+        <f t="shared" si="0"/>
         <v>2.777777777777779E-2</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
     </row>
     <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="7">
+      <c r="A67" s="6">
         <v>44693</v>
       </c>
       <c r="B67" s="5">
@@ -2284,253 +2397,253 @@
       <c r="C67" s="5">
         <v>0.34375</v>
       </c>
-      <c r="D67" s="6">
-        <f t="shared" ref="D67" si="25">C67-B67</f>
+      <c r="D67" s="16">
+        <f t="shared" si="0"/>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
+      <c r="A68" s="6"/>
       <c r="B68" s="5">
         <v>0.34375</v>
       </c>
       <c r="C68" s="5">
         <v>0.38541666666666669</v>
       </c>
-      <c r="D68" s="6">
-        <f t="shared" ref="D68:D69" si="26">C68-B68</f>
+      <c r="D68" s="16">
+        <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
+      <c r="A69" s="6"/>
       <c r="B69" s="5">
         <v>0.38541666666666669</v>
       </c>
       <c r="C69" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D69" s="6">
-        <f t="shared" si="26"/>
+      <c r="D69" s="16">
+        <f t="shared" si="0"/>
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F69" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
+      <c r="A70" s="6"/>
       <c r="B70" s="5">
         <v>0.40972222222222227</v>
       </c>
       <c r="C70" s="5">
         <v>0.4201388888888889</v>
       </c>
-      <c r="D70" s="6">
-        <f t="shared" ref="D70" si="27">C70-B70</f>
+      <c r="D70" s="16">
+        <f t="shared" ref="D70:D94" si="1">C70-B70</f>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
+      <c r="A71" s="6"/>
       <c r="B71" s="5">
         <v>0.4201388888888889</v>
       </c>
       <c r="C71" s="5">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D71" s="6">
-        <f t="shared" ref="D71" si="28">C71-B71</f>
+      <c r="D71" s="16">
+        <f t="shared" si="1"/>
         <v>5.902777777777779E-2</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F71" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
+      <c r="A72" s="6"/>
       <c r="B72" s="5">
         <v>0.47916666666666669</v>
       </c>
       <c r="C72" s="5">
         <v>0.4826388888888889</v>
       </c>
-      <c r="D72" s="6">
-        <f t="shared" ref="D72" si="29">C72-B72</f>
+      <c r="D72" s="16">
+        <f t="shared" si="1"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
+      <c r="A73" s="6"/>
       <c r="B73" s="5">
         <v>0.4826388888888889</v>
       </c>
       <c r="C73" s="5">
         <v>0.5</v>
       </c>
-      <c r="D73" s="6">
-        <f t="shared" ref="D73" si="30">C73-B73</f>
+      <c r="D73" s="16">
+        <f t="shared" si="1"/>
         <v>1.7361111111111105E-2</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F73" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G73" s="2" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
+      <c r="A74" s="6"/>
       <c r="B74" s="5">
         <v>0.5</v>
       </c>
       <c r="C74" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D74" s="6">
-        <f t="shared" ref="D74" si="31">C74-B74</f>
+      <c r="D74" s="16">
+        <f t="shared" si="1"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
+      <c r="A75" s="6"/>
       <c r="B75" s="5">
         <v>0.5625</v>
       </c>
       <c r="C75" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D75" s="6">
-        <f t="shared" ref="D75" si="32">C75-B75</f>
+      <c r="D75" s="16">
+        <f t="shared" si="1"/>
         <v>6.597222222222221E-2</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="5">
         <v>0.63888888888888895</v>
       </c>
       <c r="C76" s="5">
         <v>0.65625</v>
       </c>
-      <c r="D76" s="6">
-        <f t="shared" ref="D76" si="33">C76-B76</f>
+      <c r="D76" s="16">
+        <f t="shared" si="1"/>
         <v>1.7361111111111049E-2</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
+      <c r="A77" s="6"/>
       <c r="B77" s="5">
         <v>0.65625</v>
       </c>
       <c r="C77" s="5">
         <v>0.70486111111111116</v>
       </c>
-      <c r="D77" s="6">
-        <f t="shared" ref="D77" si="34">C77-B77</f>
+      <c r="D77" s="16">
+        <f t="shared" si="1"/>
         <v>4.861111111111116E-2</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G77" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="7">
+      <c r="A79" s="6">
         <v>44697</v>
       </c>
       <c r="B79" s="5">
@@ -2539,157 +2652,157 @@
       <c r="C79" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D79" s="6">
-        <f t="shared" ref="D79" si="35">C79-B79</f>
+      <c r="D79" s="16">
+        <f t="shared" si="1"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="7"/>
+      <c r="A80" s="6"/>
       <c r="B80" s="5">
         <v>0.41666666666666669</v>
       </c>
       <c r="C80" s="5">
         <v>0.43055555555555558</v>
       </c>
-      <c r="D80" s="6">
-        <f t="shared" ref="D80" si="36">C80-B80</f>
+      <c r="D80" s="16">
+        <f t="shared" si="1"/>
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
+      <c r="A81" s="6"/>
       <c r="B81" s="5">
         <v>0.43055555555555558</v>
       </c>
       <c r="C81" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D81" s="6">
-        <f t="shared" ref="D81" si="37">C81-B81</f>
+      <c r="D81" s="16">
+        <f t="shared" si="1"/>
         <v>7.9861111111111049E-2</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
+      <c r="A82" s="6"/>
       <c r="B82" s="5">
         <v>0.5625</v>
       </c>
       <c r="C82" s="5">
         <v>0.57291666666666663</v>
       </c>
-      <c r="D82" s="6">
-        <f t="shared" ref="D82" si="38">C82-B82</f>
+      <c r="D82" s="16">
+        <f t="shared" si="1"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G82" s="2"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
+      <c r="A83" s="6"/>
       <c r="B83" s="5">
         <v>0.57291666666666663</v>
       </c>
       <c r="C83" s="5">
         <v>0.59375</v>
       </c>
-      <c r="D83" s="6">
-        <f t="shared" ref="D83" si="39">C83-B83</f>
+      <c r="D83" s="16">
+        <f t="shared" si="1"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F83" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G83" s="2" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
+      <c r="A84" s="6"/>
       <c r="B84" s="5">
         <v>0.59375</v>
       </c>
       <c r="C84" s="5">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D84" s="6">
-        <f t="shared" ref="D84:D85" si="40">C84-B84</f>
+      <c r="D84" s="16">
+        <f t="shared" si="1"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G84" s="2"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
+      <c r="A85" s="6"/>
       <c r="B85" s="5">
         <v>0.61458333333333337</v>
       </c>
       <c r="C85" s="5">
         <v>0.62847222222222221</v>
       </c>
-      <c r="D85" s="6">
-        <f t="shared" si="40"/>
+      <c r="D85" s="16">
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="7">
+      <c r="A87" s="6">
         <v>44698</v>
       </c>
       <c r="B87" s="5">
@@ -2698,148 +2811,388 @@
       <c r="C87" s="5">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D87" s="6">
-        <f t="shared" ref="D87" si="41">C87-B87</f>
+      <c r="D87" s="16">
+        <f t="shared" si="1"/>
         <v>6.5972222222222265E-2</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G87" s="2"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="7"/>
+      <c r="A88" s="6"/>
       <c r="B88" s="5">
         <v>0.40972222222222227</v>
       </c>
       <c r="C88" s="5">
         <v>0.44097222222222227</v>
       </c>
-      <c r="D88" s="6">
-        <f t="shared" ref="D88" si="42">C88-B88</f>
+      <c r="D88" s="16">
+        <f t="shared" si="1"/>
         <v>3.125E-2</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G88" s="2" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
+      <c r="A89" s="6"/>
       <c r="B89" s="5">
         <v>0.44097222222222227</v>
       </c>
       <c r="C89" s="5">
         <v>0.4826388888888889</v>
       </c>
-      <c r="D89" s="6">
-        <f t="shared" ref="D89" si="43">C89-B89</f>
+      <c r="D89" s="16">
+        <f t="shared" si="1"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
+      <c r="A90" s="6"/>
       <c r="B90" s="5">
         <v>0.4826388888888889</v>
       </c>
       <c r="C90" s="5">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D90" s="6">
-        <f t="shared" ref="D90" si="44">C90-B90</f>
+      <c r="D90" s="16">
+        <f t="shared" si="1"/>
         <v>2.7777777777777735E-2</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F90" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G90" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G90" s="2" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
+      <c r="A91" s="6"/>
       <c r="B91" s="5">
         <v>0.5625</v>
       </c>
       <c r="C91" s="5">
         <v>0.59375</v>
       </c>
-      <c r="D91" s="6">
-        <f t="shared" ref="D91:D93" si="45">C91-B91</f>
+      <c r="D91" s="16">
+        <f t="shared" si="1"/>
         <v>3.125E-2</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F91" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G91" s="2" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
+      <c r="A92" s="6"/>
       <c r="B92" s="5">
         <v>0.59375</v>
       </c>
       <c r="C92" s="5">
         <v>0.64930555555555558</v>
       </c>
-      <c r="D92" s="6">
-        <f t="shared" si="45"/>
+      <c r="D92" s="16">
+        <f t="shared" si="1"/>
         <v>5.555555555555558E-2</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F92" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G92" s="2" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
+      <c r="A93" s="6"/>
       <c r="B93" s="5">
         <v>0.64930555555555558</v>
       </c>
       <c r="C93" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D93" s="6">
-        <f t="shared" ref="D93" si="46">C93-B93</f>
+      <c r="D93" s="16">
+        <f t="shared" si="1"/>
         <v>1.7361111111111049E-2</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>44699</v>
+      </c>
+      <c r="B94" s="5">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C94" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D94" s="16">
+        <f t="shared" si="1"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="6"/>
+      <c r="B95" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C95" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D95" s="16">
+        <f t="shared" ref="D95" si="2">C95-B95</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="6"/>
+      <c r="B96" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C96" s="5">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D96" s="16">
+        <f t="shared" ref="D96" si="3">C96-B96</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="6"/>
+      <c r="B97" s="5">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C97" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="D97" s="16">
+        <f t="shared" ref="D97" si="4">C97-B97</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="6"/>
+      <c r="B98" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="C98" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D98" s="16">
+        <f t="shared" ref="D98" si="5">C98-B98</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="6"/>
+      <c r="B99" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C99" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D99" s="16">
+        <f t="shared" ref="D99" si="6">C99-B99</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="6"/>
+      <c r="B100" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C100" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D100" s="16">
+        <f t="shared" ref="D100" si="7">C100-B100</f>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="6"/>
+      <c r="B101" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C101" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="D101" s="16">
+        <f t="shared" ref="D101" si="8">C101-B101</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="6"/>
+      <c r="B102" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="C102" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D102" s="16">
+        <f t="shared" ref="D102" si="9">C102-B102</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="6"/>
+      <c r="B103" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C103" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D103" s="16">
+        <f t="shared" ref="D103" si="10">C103-B103</f>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="6"/>
+      <c r="B104" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C104" s="5">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D104" s="16">
+        <f t="shared" ref="D104" si="11">C104-B104</f>
+        <v>3.8194444444444531E-2</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add new outing - done + some docs
</commit_message>
<xml_diff>
--- a/rapports et jdt/JdT_nithujan.xlsx
+++ b/rapports et jdt/JdT_nithujan.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPA\TPI-astronomie\rapports et jdt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\rapports et jdt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C4ABE4-17E2-4F24-91B2-DC461177FE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -567,11 +566,35 @@
   <si>
     <t>new MLD généré sans table temporaire</t>
   </si>
+  <si>
+    <t>Mise en forme du formulaire de nouvelle sortie</t>
+  </si>
+  <si>
+    <t>Gestion de la validité des données soumis via le formulaire de nouvelle sortie</t>
+  </si>
+  <si>
+    <t>Code pour l'insertion d'une nouvelle sortie</t>
+  </si>
+  <si>
+    <t>gestion des données invalides à affiner</t>
+  </si>
+  <si>
+    <t>Réussite</t>
+  </si>
+  <si>
+    <t>Relecture et ajout du MLD final</t>
+  </si>
+  <si>
+    <t>Ajout d'un message de réussite lors du login</t>
+  </si>
+  <si>
+    <t>Lorem ipsum a enlevé des pages et refaire des capture</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\ mmmm"/>
     <numFmt numFmtId="165" formatCode="[h]:mm"/>
@@ -1038,31 +1061,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="61.5546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="85.44140625" style="3" customWidth="1"/>
-    <col min="8" max="9" width="18.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="61.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="85.42578125" style="3" customWidth="1"/>
+    <col min="8" max="9" width="18.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="18" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="11.44140625" style="3"/>
+    <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>39</v>
       </c>
@@ -1073,7 +1096,7 @@
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>147</v>
       </c>
@@ -1081,13 +1104,13 @@
       <c r="D2" s="17"/>
       <c r="E2" s="13">
         <f>SUM(D5:D201)</f>
-        <v>2.7534722222222223</v>
+        <v>3.0624999999999996</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>44683</v>
       </c>
@@ -1134,7 +1157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="5">
         <v>0.41666666666666669</v>
@@ -1156,7 +1179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5">
         <v>0.5625</v>
@@ -1178,7 +1201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="5">
         <v>0.61458333333333337</v>
@@ -1200,7 +1223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1209,7 +1232,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>44684</v>
       </c>
@@ -1233,7 +1256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="5">
         <v>0.375</v>
@@ -1255,7 +1278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="5">
         <v>0.40972222222222227</v>
@@ -1277,7 +1300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="5">
         <v>0.4201388888888889</v>
@@ -1299,7 +1322,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="5">
         <v>0.4375</v>
@@ -1321,7 +1344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="5">
         <v>0.45833333333333331</v>
@@ -1343,7 +1366,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="5">
         <v>0.48958333333333331</v>
@@ -1365,7 +1388,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="5">
         <v>0.5625</v>
@@ -1387,7 +1410,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="5">
         <v>0.625</v>
@@ -1409,7 +1432,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="5">
         <v>0.63194444444444442</v>
@@ -1431,7 +1454,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="5">
         <v>0.63541666666666663</v>
@@ -1453,7 +1476,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="5">
         <v>0.64583333333333337</v>
@@ -1475,7 +1498,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="5">
         <v>0.66666666666666663</v>
@@ -1497,7 +1520,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1506,7 +1529,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>44685</v>
       </c>
@@ -1530,7 +1553,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="5">
         <v>0.40972222222222227</v>
@@ -1552,7 +1575,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="5">
         <v>0.42708333333333331</v>
@@ -1574,7 +1597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="5">
         <v>0.44791666666666669</v>
@@ -1596,7 +1619,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="5">
         <v>0.5625</v>
@@ -1618,7 +1641,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="5">
         <v>0.57291666666666663</v>
@@ -1640,7 +1663,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="5">
         <v>0.60416666666666663</v>
@@ -1662,7 +1685,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="5">
         <v>0.63888888888888895</v>
@@ -1684,7 +1707,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="5">
         <v>0.66666666666666663</v>
@@ -1706,7 +1729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="5">
         <v>0.69791666666666663</v>
@@ -1726,7 +1749,7 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1735,7 +1758,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>44686</v>
       </c>
@@ -1759,7 +1782,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="5">
         <v>0.40972222222222227</v>
@@ -1779,7 +1802,7 @@
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="5">
         <v>0.5625</v>
@@ -1801,7 +1824,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="5">
         <v>0.61111111111111105</v>
@@ -1821,7 +1844,7 @@
       </c>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="5">
         <v>0.63888888888888895</v>
@@ -1843,7 +1866,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="5">
         <v>0.67708333333333337</v>
@@ -1863,7 +1886,7 @@
       </c>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>73</v>
       </c>
@@ -1874,7 +1897,7 @@
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>44690</v>
       </c>
@@ -1898,7 +1921,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="5">
         <v>0.43055555555555558</v>
@@ -1920,7 +1943,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="5">
         <v>0.47916666666666669</v>
@@ -1942,7 +1965,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="5">
         <v>0.5</v>
@@ -1964,7 +1987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="5">
         <v>0.5625</v>
@@ -1986,7 +2009,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="5">
         <v>0.58333333333333337</v>
@@ -2008,7 +2031,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2017,7 +2040,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>44691</v>
       </c>
@@ -2041,7 +2064,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="5">
         <v>0.36458333333333331</v>
@@ -2063,7 +2086,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="5">
         <v>0.375</v>
@@ -2085,7 +2108,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="5">
         <v>0.40972222222222227</v>
@@ -2107,7 +2130,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="5">
         <v>0.41666666666666669</v>
@@ -2129,7 +2152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="5">
         <v>0.48958333333333331</v>
@@ -2151,7 +2174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="5">
         <v>0.5625</v>
@@ -2173,7 +2196,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="5">
         <v>0.63888888888888895</v>
@@ -2195,7 +2218,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="5">
         <v>0.65625</v>
@@ -2217,7 +2240,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -2226,7 +2249,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>44692</v>
       </c>
@@ -2250,7 +2273,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="5">
         <v>0.40972222222222227</v>
@@ -2272,7 +2295,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="5">
         <v>0.53125</v>
@@ -2294,7 +2317,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="5">
         <v>0.55208333333333337</v>
@@ -2316,7 +2339,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="5">
         <v>0.5625</v>
@@ -2338,7 +2361,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="5">
         <v>0.63888888888888895</v>
@@ -2360,7 +2383,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="5">
         <v>0.67708333333333337</v>
@@ -2382,7 +2405,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -2391,7 +2414,7 @@
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>44693</v>
       </c>
@@ -2415,7 +2438,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="5">
         <v>0.34375</v>
@@ -2437,7 +2460,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="5">
         <v>0.38541666666666669</v>
@@ -2459,7 +2482,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="5">
         <v>0.40972222222222227</v>
@@ -2481,7 +2504,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="5">
         <v>0.4201388888888889</v>
@@ -2503,7 +2526,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="5">
         <v>0.47916666666666669</v>
@@ -2525,7 +2548,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="5">
         <v>0.4826388888888889</v>
@@ -2547,7 +2570,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="5">
         <v>0.5</v>
@@ -2569,7 +2592,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="5">
         <v>0.5625</v>
@@ -2591,7 +2614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="5">
         <v>0.63888888888888895</v>
@@ -2613,7 +2636,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="5">
         <v>0.65625</v>
@@ -2635,7 +2658,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>123</v>
       </c>
@@ -2646,7 +2669,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>44697</v>
       </c>
@@ -2670,7 +2693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="5">
         <v>0.41666666666666669</v>
@@ -2692,7 +2715,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="5">
         <v>0.43055555555555558</v>
@@ -2714,7 +2737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="5">
         <v>0.5625</v>
@@ -2734,7 +2757,7 @@
       </c>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="5">
         <v>0.57291666666666663</v>
@@ -2756,7 +2779,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="5">
         <v>0.59375</v>
@@ -2776,7 +2799,7 @@
       </c>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="5">
         <v>0.61458333333333337</v>
@@ -2796,7 +2819,7 @@
       </c>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -2805,7 +2828,7 @@
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>44698</v>
       </c>
@@ -2825,9 +2848,11 @@
       <c r="F87" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G87" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="5">
         <v>0.40972222222222227</v>
@@ -2849,7 +2874,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="5">
         <v>0.44097222222222227</v>
@@ -2869,7 +2894,7 @@
       </c>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="5">
         <v>0.4826388888888889</v>
@@ -2891,7 +2916,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="5">
         <v>0.5625</v>
@@ -2913,7 +2938,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="5">
         <v>0.59375</v>
@@ -2935,7 +2960,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="5">
         <v>0.64930555555555558</v>
@@ -2957,7 +2982,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -2966,7 +2991,7 @@
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>44699</v>
       </c>
@@ -2988,7 +3013,7 @@
       </c>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="5">
         <v>0.375</v>
@@ -3010,7 +3035,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="5">
         <v>0.38541666666666669</v>
@@ -3032,7 +3057,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="5">
         <v>0.40972222222222227</v>
@@ -3054,7 +3079,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="5">
         <v>0.4375</v>
@@ -3076,7 +3101,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="B100" s="5">
         <v>0.47916666666666669</v>
@@ -3096,7 +3121,7 @@
       </c>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="5">
         <v>0.47916666666666669</v>
@@ -3118,7 +3143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="5">
         <v>0.5625</v>
@@ -3140,7 +3165,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="5">
         <v>0.59375</v>
@@ -3162,7 +3187,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="5">
         <v>0.63888888888888895</v>
@@ -3184,7 +3209,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="5">
         <v>0.66666666666666663</v>
@@ -3193,7 +3218,7 @@
         <v>0.70486111111111116</v>
       </c>
       <c r="D105" s="14">
-        <f t="shared" ref="D105" si="11">C105-B105</f>
+        <f t="shared" ref="D105:D107" si="11">C105-B105</f>
         <v>3.8194444444444531E-2</v>
       </c>
       <c r="E105" s="2" t="s">
@@ -3204,6 +3229,165 @@
       </c>
       <c r="G105" s="2" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="6">
+        <v>44700</v>
+      </c>
+      <c r="B107" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C107" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D107" s="14">
+        <f t="shared" si="11"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G107" s="2"/>
+    </row>
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="6"/>
+      <c r="B108" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C108" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D108" s="14">
+        <f t="shared" ref="D108" si="12">C108-B108</f>
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G108" s="2"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="6"/>
+      <c r="B109" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="C109" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D109" s="14">
+        <f t="shared" ref="D109" si="13">C109-B109</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="6"/>
+      <c r="B110" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C110" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D110" s="14">
+        <f t="shared" ref="D110" si="14">C110-B110</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="6"/>
+      <c r="B111" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C111" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D111" s="14">
+        <f t="shared" ref="D111" si="15">C111-B111</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="6"/>
+      <c r="B112" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C112" s="5">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D112" s="14">
+        <f t="shared" ref="D112" si="16">C112-B112</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G112" s="2"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="6"/>
+      <c r="B113" s="5">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C113" s="5">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D113" s="14">
+        <f t="shared" ref="D113" si="17">C113-B113</f>
+        <v>4.5138888888888951E-2</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>